<commit_message>
Courier invoice sheet changes #CRM-1203
Sub order id & product columns not required
Misc charges sheet header is wrong, it should be Misc Charges
In misc charges sheet, why are we having Product column? We have written
Service in all rows whereas we have billed all products to Partner.
Docket number to be mentioned in courier invoices sheet
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>ANNEXURE - Courier Charges</t>
   </si>
@@ -58,34 +58,28 @@
     <t>GSTIN: {meta:gst_number}</t>
   </si>
   <si>
-    <t>Sub_Order_ID</t>
-  </si>
-  <si>
     <t>Booking ID</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
+    <t>Docket Number</t>
+  </si>
+  <si>
     <t>Courier Charge</t>
   </si>
   <si>
     <t>Courier Receipt Link</t>
   </si>
   <si>
-    <t>{booking:order_id}</t>
-  </si>
-  <si>
     <t>{booking:booking_id}</t>
   </si>
   <si>
-    <t>{booking:services}</t>
-  </si>
-  <si>
     <t>{booking:city}</t>
+  </si>
+  <si>
+    <t>{booking:awb}</t>
   </si>
   <si>
     <t>{booking:courier_charges_by_sf}</t>
@@ -159,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border/>
     <border>
       <left style="thin">
@@ -168,11 +162,28 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -214,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -228,20 +239,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -250,53 +262,53 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -322,10 +334,9 @@
     <col customWidth="1" min="1" max="1" width="2.86"/>
     <col customWidth="1" min="2" max="2" width="14.43"/>
     <col customWidth="1" min="3" max="3" width="19.43"/>
-    <col customWidth="1" min="4" max="4" width="14.43"/>
-    <col customWidth="1" min="5" max="5" width="18.14"/>
-    <col customWidth="1" min="6" max="6" width="29.71"/>
-    <col customWidth="1" min="7" max="7" width="18.71"/>
+    <col customWidth="1" min="4" max="4" width="18.14"/>
+    <col customWidth="1" min="5" max="5" width="29.71"/>
+    <col customWidth="1" min="6" max="6" width="18.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -334,7 +345,6 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" ht="27.75" customHeight="1">
       <c r="A2" s="2"/>
@@ -344,215 +354,195 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="14" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="19"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="14" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="6"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="22" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="24" t="s">
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="6"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="29"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1537,12 +1527,12 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B12:D13"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
CRM-5827 Changed invoice template for partner courier(one for videocon and one for other partners)
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>ANNEXURE - Courier Charges</t>
   </si>
@@ -82,15 +82,6 @@
     <t>Booking Count</t>
   </si>
   <si>
-    <t>Total Booking Count</t>
-  </si>
-  <si>
-    <t>No of boxes</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Courier Charge</t>
   </si>
   <si>
@@ -119,15 +110,6 @@
   </si>
   <si>
     <t>{booking:count_of_booking}</t>
-  </si>
-  <si>
-    <t>{booking:p_count}</t>
-  </si>
-  <si>
-    <t>{booking:box_count}</t>
-  </si>
-  <si>
-    <t>{booking:billable_weight}</t>
   </si>
   <si>
     <t>{booking:courier_charges_by_sf}</t>
@@ -202,47 +184,17 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="19">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
     <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
     </border>
     <border>
       <left/>
@@ -351,118 +303,103 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="15" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -682,11 +619,9 @@
     <col customWidth="1" min="1" max="1" width="2.86"/>
     <col customWidth="1" min="2" max="4" width="14.43"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="10" width="13.71"/>
-    <col customWidth="1" min="11" max="12" width="11.43"/>
-    <col customWidth="1" min="13" max="13" width="20.57"/>
-    <col customWidth="1" min="14" max="14" width="18.71"/>
-    <col customWidth="1" min="15" max="26" width="8.71"/>
+    <col customWidth="1" min="6" max="9" width="13.71"/>
+    <col customWidth="1" min="10" max="10" width="20.57"/>
+    <col customWidth="1" min="11" max="11" width="18.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -700,31 +635,16 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
     </row>
     <row r="2" ht="27.75" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -733,318 +653,261 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="7"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="7"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="7"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="7"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="7"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="14"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20" t="s">
+      <c r="J10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="21"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10" t="s">
+      <c r="J11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="24"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="20" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="21"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="14"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="20" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="12"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="21"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="14"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="14"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="36" t="s">
+      <c r="J16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="34" t="s">
         <v>24</v>
-      </c>
-      <c r="L16" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" s="37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="G17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="H17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="I17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="K17" s="35" t="s">
         <v>34</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" s="38" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1053,30 +916,24 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="7"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="N19" s="42"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="39"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2061,12 +1918,12 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="B12:E13"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Revert Merge by Shubham
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>ANNEXURE - Courier Charges</t>
   </si>
@@ -82,6 +82,15 @@
     <t>Booking Count</t>
   </si>
   <si>
+    <t>Total Booking Count</t>
+  </si>
+  <si>
+    <t>No of boxes</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
     <t>Courier Charge</t>
   </si>
   <si>
@@ -110,6 +119,15 @@
   </si>
   <si>
     <t>{booking:count_of_booking}</t>
+  </si>
+  <si>
+    <t>{booking:p_count}</t>
+  </si>
+  <si>
+    <t>{booking:box_count}</t>
+  </si>
+  <si>
+    <t>{booking:billable_weight}</t>
   </si>
   <si>
     <t>{booking:courier_charges_by_sf}</t>
@@ -184,17 +202,47 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
     <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
     </border>
     <border>
       <left/>
@@ -303,103 +351,118 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="15" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="18" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -619,9 +682,11 @@
     <col customWidth="1" min="1" max="1" width="2.86"/>
     <col customWidth="1" min="2" max="4" width="14.43"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="9" width="13.71"/>
-    <col customWidth="1" min="10" max="10" width="20.57"/>
-    <col customWidth="1" min="11" max="11" width="18.71"/>
+    <col customWidth="1" min="6" max="10" width="13.71"/>
+    <col customWidth="1" min="11" max="12" width="11.43"/>
+    <col customWidth="1" min="13" max="13" width="20.57"/>
+    <col customWidth="1" min="14" max="14" width="18.71"/>
+    <col customWidth="1" min="15" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -635,16 +700,31 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" ht="27.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -653,261 +733,318 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="5"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="5"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="1"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="5"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="14"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="N10" s="21"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="11"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="1"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="N11" s="24"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="19"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="17" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="18"/>
+      <c r="N12" s="21"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="12"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="17" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="14"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="18"/>
+      <c r="N13" s="21"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="12"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="14"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="12"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="14"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="33" t="s">
+      <c r="I16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="J16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="34" t="s">
+      <c r="K16" s="36" t="s">
         <v>24</v>
+      </c>
+      <c r="L16" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="37" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="C17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="D17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="E17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="F17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="G17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="35" t="s">
+      <c r="H17" s="10" t="s">
         <v>34</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="38" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="4"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -916,24 +1053,30 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="5"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="K19" s="39"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1918,12 +2061,12 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
     <mergeCell ref="B12:E13"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Revert "Revert Merge by Shubham"
This reverts commit 9c54d2849fd20465ab36d4d4528f7d04ad5631fc.
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-courier.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>ANNEXURE - Courier Charges</t>
   </si>
@@ -82,15 +82,6 @@
     <t>Booking Count</t>
   </si>
   <si>
-    <t>Total Booking Count</t>
-  </si>
-  <si>
-    <t>No of boxes</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Courier Charge</t>
   </si>
   <si>
@@ -119,15 +110,6 @@
   </si>
   <si>
     <t>{booking:count_of_booking}</t>
-  </si>
-  <si>
-    <t>{booking:p_count}</t>
-  </si>
-  <si>
-    <t>{booking:box_count}</t>
-  </si>
-  <si>
-    <t>{booking:billable_weight}</t>
   </si>
   <si>
     <t>{booking:courier_charges_by_sf}</t>
@@ -202,47 +184,17 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="19">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
     <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
     </border>
     <border>
       <left/>
@@ -351,118 +303,103 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="15" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -682,11 +619,9 @@
     <col customWidth="1" min="1" max="1" width="2.86"/>
     <col customWidth="1" min="2" max="4" width="14.43"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="10" width="13.71"/>
-    <col customWidth="1" min="11" max="12" width="11.43"/>
-    <col customWidth="1" min="13" max="13" width="20.57"/>
-    <col customWidth="1" min="14" max="14" width="18.71"/>
-    <col customWidth="1" min="15" max="26" width="8.71"/>
+    <col customWidth="1" min="6" max="9" width="13.71"/>
+    <col customWidth="1" min="10" max="10" width="20.57"/>
+    <col customWidth="1" min="11" max="11" width="18.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -700,31 +635,16 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
     </row>
     <row r="2" ht="27.75" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -733,318 +653,261 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="7"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="7"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="7"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="7"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="7"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="14"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20" t="s">
+      <c r="J10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="21"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10" t="s">
+      <c r="J11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="24"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="20" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="21"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="14"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="20" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="12"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="21"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="14"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="14"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="36" t="s">
+      <c r="J16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="34" t="s">
         <v>24</v>
-      </c>
-      <c r="L16" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" s="37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="G17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="H17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="I17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="K17" s="35" t="s">
         <v>34</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" s="38" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1053,30 +916,24 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="7"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="N19" s="42"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="39"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2061,12 +1918,12 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="B12:E13"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>